<commit_message>
Updates template Excel file
</commit_message>
<xml_diff>
--- a/public/mal.xlsx
+++ b/public/mal.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\867_NDLA_Statistikk\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerhestad/Documents/_dev/867_NDLA_Statistikk/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE382110-F1FC-47AF-AC7E-0465963D12F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8ECF633E-719C-A049-AFA9-6AB86737FF11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13755" yWindow="1980" windowWidth="28770" windowHeight="15600"/>
+    <workbookView xWindow="13340" yWindow="3920" windowWidth="33340" windowHeight="22200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_semi" sheetId="1" r:id="rId1"/>
+    <sheet name="mal" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Januar</t>
   </si>
@@ -40,28 +51,34 @@
     <t>Måned</t>
   </si>
   <si>
-    <t>År 1</t>
-  </si>
-  <si>
-    <t>År 2</t>
-  </si>
-  <si>
-    <t>År 3</t>
-  </si>
-  <si>
-    <t>X akse</t>
-  </si>
-  <si>
-    <t>Y akse</t>
-  </si>
-  <si>
-    <t>Tonn pr. År</t>
+    <t>Aksetittel, x-akse</t>
+  </si>
+  <si>
+    <t>Aksetittel, y-akse</t>
+  </si>
+  <si>
+    <t>Tonn pr. Måned</t>
+  </si>
+  <si>
+    <t>Epler</t>
+  </si>
+  <si>
+    <t>Pærer</t>
+  </si>
+  <si>
+    <t>Bananer</t>
+  </si>
+  <si>
+    <t>Kilde</t>
+  </si>
+  <si>
+    <t>NDLA Seksjon for eksempelstatistikk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -895,112 +912,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>B1</f>
+        <v>Måned</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>123</v>
+      </c>
+      <c r="C6">
+        <v>255</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>123</v>
-      </c>
-      <c r="C5">
-        <v>255</v>
-      </c>
-      <c r="D5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>224</v>
-      </c>
-      <c r="C6">
-        <v>2345</v>
-      </c>
-      <c r="D6">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>4455</v>
       </c>
       <c r="C7">
         <v>2345</v>
       </c>
       <c r="D7">
-        <v>-1500.5</v>
+        <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>666</v>
+        <v>4455</v>
       </c>
       <c r="C8">
         <v>2345</v>
       </c>
       <c r="D8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>777</v>
+      </c>
+      <c r="C9">
+        <v>1250</v>
+      </c>
+      <c r="D9">
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>123</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>255</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>300</v>
       </c>
     </row>

</xml_diff>